<commit_message>
Fix error in formula in readme.md
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -221,9 +221,6 @@
     <t>well IDs whose 'ct' or 'drfu' is used as 'y' when constructing a straight line</t>
   </si>
   <si>
-    <t>static/test_data/ampl.xls</t>
-  </si>
-  <si>
     <t>conc</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>result</t>
+  </si>
+  <si>
+    <t>02022021.xls</t>
   </si>
 </sst>
 </file>
@@ -927,7 +927,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -983,10 +983,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
@@ -1004,7 +1004,7 @@
         <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>18</v>
@@ -1498,7 +1498,7 @@
   <dimension ref="B2:Q55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1523,7 @@
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="70"/>
       <c r="D2" s="70"/>
@@ -1582,7 +1582,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="46"/>
       <c r="E7" s="46"/>
@@ -1596,7 +1596,7 @@
         <v>42</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="46"/>
@@ -1610,7 +1610,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
@@ -1621,10 +1621,10 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="46"/>
       <c r="E10" s="46"/>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="70"/>
       <c r="D13" s="70"/>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="70"/>
       <c r="D27" s="70"/>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C49" s="70"/>
       <c r="D49" s="70"/>
@@ -2129,18 +2129,18 @@
   <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="78"/>
       <c r="E2" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F2" s="78"/>
     </row>
@@ -2149,34 +2149,34 @@
         <v>23</v>
       </c>
       <c r="C3" s="68">
-        <v>15</v>
+        <v>27.6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3">
         <f>10^((C3-C7)/C5)</f>
-        <v>2.6176431902199688</v>
+        <v>4.5364530228690425E-4</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="68">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="3">
         <f>F3*LN(10)/ABS(C5)*C11</f>
-        <v>0.80029680007135595</v>
+        <v>1.9369792893712064E-4</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="68">
         <v>-3.35</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="68">
         <v>0.13</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="68">
         <v>16.399999999999999</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="68">
         <v>0.43</v>
@@ -2208,17 +2208,17 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="78"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="67">
         <f>SQRT(C4^2+C8^2+(C6*(C3-C7)/C5)^2)</f>
-        <v>0.44480509271554042</v>
+        <v>0.62120891201234019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>